<commit_message>
Added the sorting list per department, added it to the DataFrame and sorted it
</commit_message>
<xml_diff>
--- a/Resources/Picard_end_credit.xlsx
+++ b/Resources/Picard_end_credit.xlsx
@@ -25,244 +25,244 @@
     <t>VFX SUPERVISOR</t>
   </si>
   <si>
+    <t>LEAD COMPOSITOR</t>
+  </si>
+  <si>
+    <t>COMPOSITOR</t>
+  </si>
+  <si>
+    <t>CG SUPERVISOR</t>
+  </si>
+  <si>
     <t>TD LIGHTING</t>
   </si>
   <si>
+    <t>MATTE PAINTER</t>
+  </si>
+  <si>
+    <t>FX SUPERVISOR</t>
+  </si>
+  <si>
+    <t>FX ARTIST</t>
+  </si>
+  <si>
+    <t>LEAD ANIMATOR</t>
+  </si>
+  <si>
+    <t>TD RIGGER</t>
+  </si>
+  <si>
+    <t>OUTSOURCE</t>
+  </si>
+  <si>
     <t>TBD</t>
   </si>
   <si>
-    <t>FX ARTIST</t>
-  </si>
-  <si>
-    <t>CG SUPERVISOR</t>
-  </si>
-  <si>
-    <t>TD RIGGER</t>
-  </si>
-  <si>
-    <t>LEAD COMPOSITOR</t>
-  </si>
-  <si>
-    <t>OUTSOURCE</t>
-  </si>
-  <si>
-    <t>LEAD ANIMATOR</t>
-  </si>
-  <si>
-    <t>COMPOSITOR</t>
-  </si>
-  <si>
-    <t>FX SUPERVISOR</t>
-  </si>
-  <si>
-    <t>MATTE PAINTER</t>
-  </si>
-  <si>
     <t>RICK RAMIREZ</t>
   </si>
   <si>
+    <t>RYAN SMOLAREK</t>
+  </si>
+  <si>
+    <t>DAVID SILVA</t>
+  </si>
+  <si>
+    <t>NICK DODGE</t>
+  </si>
+  <si>
+    <t>KIMBERLY MARTINEZ</t>
+  </si>
+  <si>
+    <t>KENNEY KIMBLE</t>
+  </si>
+  <si>
+    <t>JAVIER GALLEGO</t>
+  </si>
+  <si>
+    <t>ALEXIS TARAKJIAN</t>
+  </si>
+  <si>
+    <t>DAVID HOCHSTADTER</t>
+  </si>
+  <si>
+    <t>ELIZABETH BODNAR</t>
+  </si>
+  <si>
+    <t>ERIK O' DONNELL</t>
+  </si>
+  <si>
+    <t>STEVE GRAVES</t>
+  </si>
+  <si>
     <t>YINGLEI YANG</t>
   </si>
   <si>
+    <t>MAYUMI SHIMOKAWA</t>
+  </si>
+  <si>
+    <t>RIGEL BOWEN</t>
+  </si>
+  <si>
+    <t>SEUNG LEE</t>
+  </si>
+  <si>
+    <t>VLAD TUSHEVSKIY</t>
+  </si>
+  <si>
+    <t>JASON SHULMAN</t>
+  </si>
+  <si>
+    <t>ANDREI OREHOV</t>
+  </si>
+  <si>
+    <t>YANNIX</t>
+  </si>
+  <si>
+    <t>ROTOMAKER</t>
+  </si>
+  <si>
+    <t>VFX TRACKING</t>
+  </si>
+  <si>
+    <t>RHINESTONEVFX</t>
+  </si>
+  <si>
+    <t>HEATHER FETTER</t>
+  </si>
+  <si>
+    <t>LUIS CAYO</t>
+  </si>
+  <si>
+    <t>BADNAMED-KIM SYBERG</t>
+  </si>
+  <si>
+    <t>KRIS KELLY</t>
+  </si>
+  <si>
+    <t>MICHAEL DE LORENZO</t>
+  </si>
+  <si>
+    <t>RICHARD MAHON</t>
+  </si>
+  <si>
+    <t>BRANDON MACDOUGALL</t>
+  </si>
+  <si>
+    <t>MIKE KRUEGER</t>
+  </si>
+  <si>
+    <t>HOLLY WENGER</t>
+  </si>
+  <si>
+    <t>DOUG WITSKEN</t>
+  </si>
+  <si>
+    <t>TIM SIMON</t>
+  </si>
+  <si>
+    <t>DANIEL FLORES</t>
+  </si>
+  <si>
     <t>CHRIS PIERZ</t>
   </si>
   <si>
-    <t>VLAD TUSHEVSKIY</t>
+    <t>BUDDY GHEEN</t>
+  </si>
+  <si>
+    <t>JON GOURLEY</t>
+  </si>
+  <si>
+    <t>JONATHAN BLISS</t>
+  </si>
+  <si>
+    <t>BRANDON YOUNG</t>
+  </si>
+  <si>
+    <t>DAN APREA</t>
+  </si>
+  <si>
+    <t>SARAH LOPEZ</t>
+  </si>
+  <si>
+    <t>PATRICIO HARRIS</t>
+  </si>
+  <si>
+    <t>BRUCE COY</t>
+  </si>
+  <si>
+    <t>ALEXEY CHEPRAKOV</t>
+  </si>
+  <si>
+    <t>FRANK SYNOWICZ</t>
+  </si>
+  <si>
+    <t>FORREST ARNOLD</t>
+  </si>
+  <si>
+    <t>DAVID NELSON</t>
+  </si>
+  <si>
+    <t>NICK SINNOTT</t>
+  </si>
+  <si>
+    <t>CHRISTOPHER KNIGHT</t>
+  </si>
+  <si>
+    <t>PETER HERLEIN</t>
+  </si>
+  <si>
+    <t>SLAVA PONOMAREV</t>
+  </si>
+  <si>
+    <t>JACOB COY</t>
+  </si>
+  <si>
+    <t>DANIEL FAZEL</t>
+  </si>
+  <si>
+    <t>EDITH CLARA</t>
+  </si>
+  <si>
+    <t>VIT ZELICH</t>
+  </si>
+  <si>
+    <t>DAVID GUTMAN</t>
+  </si>
+  <si>
+    <t>THOMAS MAINE</t>
+  </si>
+  <si>
+    <t>DUSTIN ADAIR</t>
   </si>
   <si>
     <t>WILLIAM MAUER</t>
   </si>
   <si>
-    <t>STEVE GRAVES</t>
-  </si>
-  <si>
-    <t>ANDREI OREHOV</t>
-  </si>
-  <si>
-    <t>DAVID GUTMAN</t>
-  </si>
-  <si>
-    <t>DAVID SILVA</t>
-  </si>
-  <si>
-    <t>JONATHAN BLISS</t>
-  </si>
-  <si>
-    <t>JON GOURLEY</t>
-  </si>
-  <si>
-    <t>ROTOMAKER</t>
-  </si>
-  <si>
-    <t>JASON SHULMAN</t>
-  </si>
-  <si>
-    <t>ALEXEY CHEPRAKOV</t>
-  </si>
-  <si>
-    <t>RYAN SMOLAREK</t>
+    <t>BRIAN DAVIS</t>
+  </si>
+  <si>
+    <t>GARY LOPEZ</t>
+  </si>
+  <si>
+    <t>TONY CASTRO</t>
   </si>
   <si>
     <t>VAL KHARITONASHVILI</t>
   </si>
   <si>
-    <t>VFX TRACKING</t>
-  </si>
-  <si>
-    <t>BRUCE COY</t>
-  </si>
-  <si>
-    <t>GARY LOPEZ</t>
-  </si>
-  <si>
-    <t>FORREST ARNOLD</t>
-  </si>
-  <si>
-    <t>RHINESTONEVFX</t>
-  </si>
-  <si>
-    <t>NICK SINNOTT</t>
-  </si>
-  <si>
-    <t>PATRICIO HARRIS</t>
-  </si>
-  <si>
-    <t>DUSTIN ADAIR</t>
-  </si>
-  <si>
-    <t>PETER HERLEIN</t>
-  </si>
-  <si>
-    <t>YANNIX</t>
-  </si>
-  <si>
-    <t>ELIZABETH BODNAR</t>
-  </si>
-  <si>
-    <t>SLAVA PONOMAREV</t>
-  </si>
-  <si>
-    <t>DANIEL FAZEL</t>
-  </si>
-  <si>
-    <t>JACOB COY</t>
-  </si>
-  <si>
-    <t>JAVIER GALLEGO</t>
-  </si>
-  <si>
-    <t>EDITH CLARA</t>
-  </si>
-  <si>
-    <t>TIM SIMON</t>
-  </si>
-  <si>
-    <t>CHRISTOPHER KNIGHT</t>
-  </si>
-  <si>
-    <t>ALEXIS TARAKJIAN</t>
-  </si>
-  <si>
-    <t>HOLLY WENGER</t>
+    <t>KEN BRILLIANT</t>
+  </si>
+  <si>
+    <t>JOSH MOSSOTTI</t>
   </si>
   <si>
     <t>SEAN COX</t>
   </si>
   <si>
-    <t>VIT ZELICH</t>
-  </si>
-  <si>
-    <t>DAVID NELSON</t>
-  </si>
-  <si>
-    <t>ERIK O' DONNELL</t>
-  </si>
-  <si>
-    <t>RIGEL BOWEN</t>
-  </si>
-  <si>
-    <t>TONY CASTRO</t>
-  </si>
-  <si>
-    <t>KEN BRILLIANT</t>
-  </si>
-  <si>
-    <t>DAVID HOCHSTADTER</t>
-  </si>
-  <si>
-    <t>DAN APREA</t>
-  </si>
-  <si>
-    <t>JOSH MOSSOTTI</t>
-  </si>
-  <si>
-    <t>MIKE KRUEGER</t>
-  </si>
-  <si>
-    <t>DANIEL FLORES</t>
-  </si>
-  <si>
-    <t>SARAH LOPEZ</t>
-  </si>
-  <si>
-    <t>HEATHER FETTER</t>
-  </si>
-  <si>
-    <t>KIMBERLY MARTINEZ</t>
-  </si>
-  <si>
-    <t>NICK DODGE</t>
-  </si>
-  <si>
-    <t>MICHAEL DE LORENZO</t>
-  </si>
-  <si>
-    <t>FRANK SYNOWICZ</t>
-  </si>
-  <si>
-    <t>SEUNG LEE</t>
-  </si>
-  <si>
-    <t>RICHARD MAHON</t>
-  </si>
-  <si>
-    <t>BRANDON MACDOUGALL</t>
-  </si>
-  <si>
-    <t>BRIAN DAVIS</t>
-  </si>
-  <si>
-    <t>DOUG WITSKEN</t>
-  </si>
-  <si>
-    <t>LUIS CAYO</t>
-  </si>
-  <si>
-    <t>MAYUMI SHIMOKAWA</t>
-  </si>
-  <si>
-    <t>BRANDON YOUNG</t>
-  </si>
-  <si>
-    <t>KRIS KELLY</t>
-  </si>
-  <si>
-    <t>BADNAMED-KIM SYBERG</t>
-  </si>
-  <si>
-    <t>KENNEY KIMBLE</t>
-  </si>
-  <si>
-    <t>THOMAS MAINE</t>
-  </si>
-  <si>
-    <t>BUDDY GHEEN</t>
-  </si>
-  <si>
     <t>Remark:</t>
   </si>
   <si>
-    <t>The last update time is 21:53.</t>
+    <t>The last update time is 09:27.</t>
   </si>
 </sst>
 </file>
@@ -669,35 +669,35 @@
     </row>
     <row r="6" spans="2:10">
       <c r="D6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="J6" s="1">
-        <v>238</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:10">
       <c r="D7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="1">
-        <v>220</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="D8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
       <c r="J8" s="1">
-        <v>215</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -708,29 +708,29 @@
         <v>18</v>
       </c>
       <c r="J9" s="1">
-        <v>197</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="1">
-        <v>178</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
       </c>
       <c r="J11" s="1">
-        <v>150</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:10">
@@ -741,18 +741,18 @@
         <v>21</v>
       </c>
       <c r="J12" s="1">
-        <v>139</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:10">
       <c r="D13" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
         <v>22</v>
       </c>
       <c r="J13" s="1">
-        <v>98</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:10">
@@ -763,7 +763,7 @@
         <v>23</v>
       </c>
       <c r="J14" s="1">
-        <v>92</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:10">
@@ -774,62 +774,62 @@
         <v>24</v>
       </c>
       <c r="J15" s="1">
-        <v>73</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:10">
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
       </c>
       <c r="J16" s="1">
-        <v>69</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="4:10">
       <c r="D17" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="1">
-        <v>60</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="4:10">
       <c r="D18" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
         <v>27</v>
       </c>
       <c r="J18" s="1">
-        <v>56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="4:10">
       <c r="D19" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
         <v>28</v>
       </c>
       <c r="J19" s="1">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:10">
       <c r="D20" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
         <v>29</v>
       </c>
       <c r="J20" s="1">
-        <v>51</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="4:10">
@@ -840,188 +840,188 @@
         <v>30</v>
       </c>
       <c r="J21" s="1">
-        <v>42</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="4:10">
       <c r="D22" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
         <v>31</v>
       </c>
       <c r="J22" s="1">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="4:10">
       <c r="D23" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
         <v>32</v>
       </c>
       <c r="J23" s="1">
-        <v>36</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="4:10">
       <c r="D24" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
         <v>33</v>
       </c>
       <c r="J24" s="1">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="4:10">
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
         <v>34</v>
       </c>
       <c r="J25" s="1">
-        <v>31</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="4:10">
       <c r="D26" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
         <v>35</v>
       </c>
       <c r="J26" s="1">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="4:10">
       <c r="D27" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
         <v>36</v>
       </c>
       <c r="J27" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="4:10">
       <c r="D28" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
         <v>37</v>
       </c>
       <c r="J28" s="1">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="4:10">
       <c r="D29" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
         <v>38</v>
       </c>
       <c r="J29" s="1">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="4:10">
       <c r="D30" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
         <v>39</v>
       </c>
       <c r="J30" s="1">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="4:10">
       <c r="D31" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
         <v>40</v>
       </c>
       <c r="J31" s="1">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="4:10">
       <c r="D32" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
         <v>41</v>
       </c>
       <c r="J32" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="4:10">
       <c r="D33" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
         <v>42</v>
       </c>
       <c r="J33" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="4:10">
       <c r="D34" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F34" t="s">
         <v>43</v>
       </c>
       <c r="J34" s="1">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="4:10">
       <c r="D35" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
         <v>44</v>
       </c>
       <c r="J35" s="1">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="4:10">
       <c r="D36" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F36" t="s">
         <v>45</v>
       </c>
       <c r="J36" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="4:10">
       <c r="D37" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
         <v>46</v>
       </c>
       <c r="J37" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="4:10">
       <c r="D38" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
         <v>47</v>
@@ -1032,73 +1032,73 @@
     </row>
     <row r="39" spans="4:10">
       <c r="D39" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F39" t="s">
         <v>48</v>
       </c>
       <c r="J39" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="4:10">
       <c r="D40" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
         <v>49</v>
       </c>
       <c r="J40" s="1">
-        <v>8</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="4:10">
       <c r="D41" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F41" t="s">
         <v>50</v>
       </c>
       <c r="J41" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="4:10">
       <c r="D42" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F42" t="s">
         <v>51</v>
       </c>
       <c r="J42" s="1">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="4:10">
       <c r="D43" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F43" t="s">
         <v>52</v>
       </c>
       <c r="J43" s="1">
-        <v>7</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="4:10">
       <c r="D44" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F44" t="s">
         <v>53</v>
       </c>
       <c r="J44" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="4:10">
       <c r="D45" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F45" t="s">
         <v>54</v>
@@ -1109,211 +1109,211 @@
     </row>
     <row r="46" spans="4:10">
       <c r="D46" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F46" t="s">
         <v>55</v>
       </c>
       <c r="J46" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="4:10">
       <c r="D47" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
         <v>56</v>
       </c>
       <c r="J47" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="4:10">
       <c r="D48" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F48" t="s">
         <v>57</v>
       </c>
       <c r="J48" s="1">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="4:10">
       <c r="D49" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F49" t="s">
         <v>58</v>
       </c>
       <c r="J49" s="1">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="4:10">
       <c r="D50" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
         <v>59</v>
       </c>
       <c r="J50" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="4:10">
       <c r="D51" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F51" t="s">
         <v>60</v>
       </c>
       <c r="J51" s="1">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="4:10">
       <c r="D52" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F52" t="s">
         <v>61</v>
       </c>
       <c r="J52" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="4:10">
       <c r="D53" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F53" t="s">
         <v>62</v>
       </c>
       <c r="J53" s="1">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="4:10">
       <c r="D54" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F54" t="s">
         <v>63</v>
       </c>
       <c r="J54" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="4:10">
       <c r="D55" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F55" t="s">
         <v>64</v>
       </c>
       <c r="J55" s="1">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="4:10">
       <c r="D56" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F56" t="s">
         <v>65</v>
       </c>
       <c r="J56" s="1">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="57" spans="4:10">
       <c r="D57" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F57" t="s">
         <v>66</v>
       </c>
       <c r="J57" s="1">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="4:10">
       <c r="D58" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F58" t="s">
         <v>67</v>
       </c>
       <c r="J58" s="1">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="4:10">
       <c r="D59" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F59" t="s">
         <v>68</v>
       </c>
       <c r="J59" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="4:10">
       <c r="D60" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F60" t="s">
         <v>69</v>
       </c>
       <c r="J60" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="4:10">
       <c r="D61" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F61" t="s">
         <v>70</v>
       </c>
       <c r="J61" s="1">
-        <v>2</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="4:10">
       <c r="D62" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F62" t="s">
         <v>71</v>
       </c>
       <c r="J62" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="4:10">
       <c r="D63" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F63" t="s">
         <v>72</v>
       </c>
       <c r="J63" s="1">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="4:10">
       <c r="D64" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F64" t="s">
         <v>73</v>
       </c>
       <c r="J64" s="1">
-        <v>2</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -1324,73 +1324,73 @@
         <v>74</v>
       </c>
       <c r="J65" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="D66" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F66" t="s">
         <v>75</v>
       </c>
       <c r="J66" s="1">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="D67" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F67" t="s">
         <v>76</v>
       </c>
       <c r="J67" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="D68" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F68" t="s">
         <v>77</v>
       </c>
       <c r="J68" s="1">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="D69" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F69" t="s">
         <v>78</v>
       </c>
       <c r="J69" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="D70" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F70" t="s">
         <v>79</v>
       </c>
       <c r="J70" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="D71" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F71" t="s">
         <v>80</v>
       </c>
       <c r="J71" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:10">

</xml_diff>

<commit_message>
Concat a new json file with DataFrame to unclude the support team in the generic
</commit_message>
<xml_diff>
--- a/Resources/Picard_end_credit.xlsx
+++ b/Resources/Picard_end_credit.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="99">
   <si>
     <t>GHOST VFX</t>
   </si>
@@ -25,6 +25,12 @@
     <t>VFX SUPERVISOR</t>
   </si>
   <si>
+    <t>EXECUTIVE PRODUCER</t>
+  </si>
+  <si>
+    <t>COORDINATOR</t>
+  </si>
+  <si>
     <t>COMPOSITING SUPERVISOR</t>
   </si>
   <si>
@@ -67,6 +73,12 @@
     <t>TD RIGGER</t>
   </si>
   <si>
+    <t>VFX EDITORIAL MANAGER</t>
+  </si>
+  <si>
+    <t>VFX EDITOR</t>
+  </si>
+  <si>
     <t>PIPELINE SUPERVISOR</t>
   </si>
   <si>
@@ -82,16 +94,31 @@
     <t>RYAN SMOLAREK</t>
   </si>
   <si>
+    <t>SARAH MCGRAIL</t>
+  </si>
+  <si>
+    <t>ANNA WHOLEY</t>
+  </si>
+  <si>
     <t>SEAN COX</t>
   </si>
   <si>
     <t>DAVID SILVA</t>
   </si>
   <si>
+    <t>GARY LOPEZ</t>
+  </si>
+  <si>
+    <t>PETER HERLEIN</t>
+  </si>
+  <si>
     <t>ELIZABETH BODNAR</t>
   </si>
   <si>
-    <t>PETER HERLEIN</t>
+    <t>JACOB COY</t>
+  </si>
+  <si>
+    <t>JAVIER GALLEGO</t>
   </si>
   <si>
     <t>ALEXIS TARAKJIAN</t>
@@ -100,22 +127,16 @@
     <t>ERIK O' DONNELL</t>
   </si>
   <si>
-    <t>GARY LOPEZ</t>
-  </si>
-  <si>
     <t>TONY CASTRO</t>
   </si>
   <si>
     <t>DAVID HOCHSTADTER</t>
   </si>
   <si>
-    <t>JACOB COY</t>
-  </si>
-  <si>
     <t>DANIEL FLORES</t>
   </si>
   <si>
-    <t>JAVIER GALLEGO</t>
+    <t>HEATHER FETTER</t>
   </si>
   <si>
     <t>KIMBERLY MARTINEZ</t>
@@ -127,160 +148,169 @@
     <t>KENNEY KIMBLE</t>
   </si>
   <si>
-    <t>HEATHER FETTER</t>
+    <t>STEVE GRAVES</t>
   </si>
   <si>
     <t>THOMAS MAINE</t>
   </si>
   <si>
-    <t>STEVE GRAVES</t>
+    <t>YINGLEI YANG</t>
+  </si>
+  <si>
+    <t>DAVID GUTMAN</t>
+  </si>
+  <si>
+    <t>PATRICIO HARRIS</t>
   </si>
   <si>
     <t>SLAVA PONOMAREV</t>
   </si>
   <si>
-    <t>YINGLEI YANG</t>
-  </si>
-  <si>
-    <t>PATRICIO HARRIS</t>
-  </si>
-  <si>
-    <t>DAVID GUTMAN</t>
+    <t>RICHARD MAHON</t>
   </si>
   <si>
     <t>MAYUMI SHIMOKAWA</t>
   </si>
   <si>
-    <t>RICHARD MAHON</t>
+    <t>CHRIS PIERZ</t>
+  </si>
+  <si>
+    <t>WILLIAM MAUER</t>
+  </si>
+  <si>
+    <t>JONATHAN BLISS</t>
+  </si>
+  <si>
+    <t>JON GOURLEY</t>
+  </si>
+  <si>
+    <t>BRUCE COY</t>
+  </si>
+  <si>
+    <t>FORREST ARNOLD</t>
+  </si>
+  <si>
+    <t>DANIEL FAZEL</t>
+  </si>
+  <si>
+    <t>TIM SIMON</t>
   </si>
   <si>
     <t>VIT ZELICH</t>
   </si>
   <si>
+    <t>DAN APREA</t>
+  </si>
+  <si>
     <t>FRANK SYNOWICZ</t>
   </si>
   <si>
-    <t>TIM SIMON</t>
-  </si>
-  <si>
     <t>LUIS CAYO</t>
   </si>
   <si>
-    <t>DAN APREA</t>
-  </si>
-  <si>
     <t>BUDDY GHEEN</t>
   </si>
   <si>
-    <t>DANIEL FAZEL</t>
-  </si>
-  <si>
-    <t>CHRIS PIERZ</t>
-  </si>
-  <si>
-    <t>WILLIAM MAUER</t>
-  </si>
-  <si>
-    <t>JONATHAN BLISS</t>
-  </si>
-  <si>
-    <t>FORREST ARNOLD</t>
-  </si>
-  <si>
-    <t>BRUCE COY</t>
-  </si>
-  <si>
-    <t>JON GOURLEY</t>
-  </si>
-  <si>
     <t>RIGEL BOWEN</t>
   </si>
   <si>
     <t>VLAD TUSHEVSKIY</t>
   </si>
   <si>
+    <t>ALEXEY CHEPRAKOV</t>
+  </si>
+  <si>
+    <t>VAL KHARITONASHVILI</t>
+  </si>
+  <si>
+    <t>MIKE KRUEGER</t>
+  </si>
+  <si>
+    <t>SEUNG LEE</t>
+  </si>
+  <si>
     <t>BRIAN DAVIS</t>
   </si>
   <si>
-    <t>SEUNG LEE</t>
-  </si>
-  <si>
-    <t>ALEXEY CHEPRAKOV</t>
-  </si>
-  <si>
-    <t>VAL KHARITONASHVILI</t>
-  </si>
-  <si>
-    <t>MIKE KRUEGER</t>
-  </si>
-  <si>
     <t>JASON SHULMAN</t>
   </si>
   <si>
+    <t>DUSTIN ADAIR</t>
+  </si>
+  <si>
+    <t>KEN BRILLIANT</t>
+  </si>
+  <si>
     <t>KRIS KELLY</t>
   </si>
   <si>
-    <t>KEN BRILLIANT</t>
-  </si>
-  <si>
-    <t>DUSTIN ADAIR</t>
-  </si>
-  <si>
     <t>HOLLY WENGER</t>
   </si>
   <si>
+    <t>NICK SINNOTT</t>
+  </si>
+  <si>
     <t>EDITH CLARA</t>
   </si>
   <si>
-    <t>NICK SINNOTT</t>
-  </si>
-  <si>
     <t>ANDREI OREHOV</t>
   </si>
   <si>
+    <t>MIGUEL RUSTIA</t>
+  </si>
+  <si>
+    <t>EDUARDO CISNEROS</t>
+  </si>
+  <si>
+    <t>PAUL STEMMER</t>
+  </si>
+  <si>
+    <t>ANDREW JUPINA</t>
+  </si>
+  <si>
     <t>CHRISTOPHER KNIGHT</t>
   </si>
   <si>
     <t>MICHAEL DE LORENZO</t>
   </si>
   <si>
+    <t>ROTOMAKER</t>
+  </si>
+  <si>
+    <t>VFX TRACKING</t>
+  </si>
+  <si>
+    <t>RHINESTONEVFX</t>
+  </si>
+  <si>
     <t>YANNIX</t>
   </si>
   <si>
-    <t>VFX TRACKING</t>
-  </si>
-  <si>
-    <t>RHINESTONEVFX</t>
-  </si>
-  <si>
-    <t>ROTOMAKER</t>
+    <t>DAVID NELSON</t>
+  </si>
+  <si>
+    <t>JOSH MOSSOTTI</t>
+  </si>
+  <si>
+    <t>SARAH LOPEZ</t>
+  </si>
+  <si>
+    <t>BRANDON MACDOUGALL</t>
   </si>
   <si>
     <t>DOUG WITSKEN</t>
   </si>
   <si>
-    <t>DAVID NELSON</t>
-  </si>
-  <si>
     <t>BRANDON YOUNG</t>
   </si>
   <si>
     <t>BADNAMED-KIM SYBERG</t>
   </si>
   <si>
-    <t>SARAH LOPEZ</t>
-  </si>
-  <si>
-    <t>JOSH MOSSOTTI</t>
-  </si>
-  <si>
-    <t>BRANDON MACDOUGALL</t>
-  </si>
-  <si>
     <t>For Internal Use Only</t>
   </si>
   <si>
-    <t>Last update time 23:42.</t>
+    <t>Last update time 23:19.</t>
   </si>
 </sst>
 </file>
@@ -690,7 +720,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -751,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H5" s="6"/>
       <c r="J5" s="2">
@@ -764,7 +794,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H6" s="6"/>
       <c r="J6" s="2">
@@ -777,11 +807,11 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H7" s="6"/>
       <c r="J7" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -790,11 +820,11 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H8" s="6"/>
       <c r="J8" s="2">
-        <v>98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -803,176 +833,176 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H9" s="6"/>
       <c r="J9" s="2">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="4"/>
       <c r="D10" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H10" s="6"/>
       <c r="J10" s="2">
-        <v>23</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="4"/>
       <c r="D11" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H11" s="6"/>
       <c r="J11" s="2">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="4"/>
       <c r="D12" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H12" s="6"/>
       <c r="J12" s="2">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H13" s="6"/>
       <c r="J13" s="2">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="4"/>
       <c r="D14" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H14" s="6"/>
       <c r="J14" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:10">
       <c r="B15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H15" s="6"/>
       <c r="J15" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="4"/>
       <c r="D16" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H16" s="6"/>
       <c r="J16" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="4"/>
       <c r="D17" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H17" s="6"/>
       <c r="J17" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="4"/>
       <c r="D18" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H18" s="6"/>
       <c r="J18" s="2">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:10">
       <c r="B19" s="4"/>
       <c r="D19" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H19" s="6"/>
       <c r="J19" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="4"/>
       <c r="D20" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H20" s="6"/>
       <c r="J20" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="B21" s="4"/>
       <c r="D21" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H21" s="6"/>
       <c r="J21" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="4"/>
       <c r="D22" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H22" s="6"/>
       <c r="J22" s="2">
@@ -982,75 +1012,75 @@
     <row r="23" spans="2:10">
       <c r="B23" s="4"/>
       <c r="D23" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H23" s="6"/>
       <c r="J23" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:10">
       <c r="B24" s="4"/>
       <c r="D24" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H24" s="6"/>
       <c r="J24" s="2">
-        <v>178</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="4"/>
       <c r="D25" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H25" s="6"/>
       <c r="J25" s="2">
-        <v>16</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="4"/>
       <c r="D26" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H26" s="6"/>
       <c r="J26" s="2">
-        <v>238</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="4"/>
       <c r="D27" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H27" s="6"/>
       <c r="J27" s="2">
-        <v>27</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="4"/>
       <c r="D28" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H28" s="6"/>
       <c r="J28" s="2">
@@ -1060,209 +1090,209 @@
     <row r="29" spans="2:10">
       <c r="B29" s="4"/>
       <c r="D29" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H29" s="6"/>
       <c r="J29" s="2">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="4"/>
       <c r="D30" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H30" s="6"/>
       <c r="J30" s="2">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="4"/>
       <c r="D31" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H31" s="6"/>
       <c r="J31" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="4"/>
       <c r="D32" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H32" s="6"/>
       <c r="J32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="4"/>
       <c r="D33" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H33" s="6"/>
       <c r="J33" s="2">
-        <v>9</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="4"/>
       <c r="D34" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H34" s="6"/>
       <c r="J34" s="2">
-        <v>2</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="4"/>
       <c r="D35" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H35" s="6"/>
       <c r="J35" s="2">
-        <v>5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="4"/>
       <c r="D36" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H36" s="6"/>
       <c r="J36" s="2">
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="4"/>
       <c r="D37" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H37" s="6"/>
       <c r="J37" s="2">
-        <v>16</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="4"/>
       <c r="D38" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H38" s="6"/>
       <c r="J38" s="2">
-        <v>220</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="4"/>
       <c r="D39" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H39" s="6"/>
       <c r="J39" s="2">
-        <v>197</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="2:10">
       <c r="B40" s="4"/>
       <c r="D40" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H40" s="6"/>
       <c r="J40" s="2">
-        <v>92</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="4"/>
       <c r="D41" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H41" s="6"/>
       <c r="J41" s="2">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="2:10">
       <c r="B42" s="4"/>
       <c r="D42" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F42" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H42" s="6"/>
       <c r="J42" s="2">
-        <v>41</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="2:10">
       <c r="B43" s="4"/>
       <c r="D43" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F43" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H43" s="6"/>
       <c r="J43" s="2">
-        <v>73</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="4"/>
       <c r="D44" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F44" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H44" s="6"/>
       <c r="J44" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="2:10">
@@ -1271,46 +1301,46 @@
         <v>11</v>
       </c>
       <c r="F45" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H45" s="6"/>
       <c r="J45" s="2">
-        <v>215</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:10">
       <c r="B46" s="4"/>
       <c r="D46" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H46" s="6"/>
       <c r="J46" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="2:10">
       <c r="B47" s="4"/>
       <c r="D47" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H47" s="6"/>
       <c r="J47" s="2">
-        <v>2</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="2:10">
       <c r="B48" s="4"/>
       <c r="D48" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F48" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H48" s="6"/>
       <c r="J48" s="2">
@@ -1320,10 +1350,10 @@
     <row r="49" spans="2:10">
       <c r="B49" s="4"/>
       <c r="D49" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F49" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H49" s="6"/>
       <c r="J49" s="2">
@@ -1333,10 +1363,10 @@
     <row r="50" spans="2:10">
       <c r="B50" s="4"/>
       <c r="D50" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F50" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H50" s="6"/>
       <c r="J50" s="2">
@@ -1346,14 +1376,14 @@
     <row r="51" spans="2:10">
       <c r="B51" s="4"/>
       <c r="D51" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F51" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H51" s="6"/>
       <c r="J51" s="2">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="2:10">
@@ -1362,33 +1392,33 @@
         <v>13</v>
       </c>
       <c r="F52" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H52" s="6"/>
       <c r="J52" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="2:10">
       <c r="B53" s="4"/>
       <c r="D53" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F53" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H53" s="6"/>
       <c r="J53" s="2">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="2:10">
       <c r="B54" s="4"/>
       <c r="D54" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H54" s="6"/>
       <c r="J54" s="2">
@@ -1398,14 +1428,14 @@
     <row r="55" spans="2:10">
       <c r="B55" s="4"/>
       <c r="D55" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H55" s="6"/>
       <c r="J55" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="2:10">
@@ -1414,37 +1444,37 @@
         <v>15</v>
       </c>
       <c r="F56" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H56" s="6"/>
       <c r="J56" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="2:10">
       <c r="B57" s="4"/>
       <c r="D57" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F57" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H57" s="6"/>
       <c r="J57" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="2:10">
       <c r="B58" s="4"/>
       <c r="D58" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F58" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H58" s="6"/>
       <c r="J58" s="2">
-        <v>150</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="2:10">
@@ -1453,7 +1483,7 @@
         <v>17</v>
       </c>
       <c r="F59" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H59" s="6"/>
       <c r="J59" s="2">
@@ -1463,177 +1493,254 @@
     <row r="60" spans="2:10">
       <c r="B60" s="4"/>
       <c r="D60" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F60" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H60" s="6"/>
       <c r="J60" s="2">
-        <v>3</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="2:10">
       <c r="B61" s="4"/>
       <c r="D61" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F61" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H61" s="6"/>
       <c r="J61" s="2">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:10">
       <c r="B62" s="4"/>
       <c r="D62" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H62" s="6"/>
       <c r="J62" s="2">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:10">
       <c r="B63" s="4"/>
       <c r="D63" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H63" s="6"/>
       <c r="J63" s="2">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:10">
       <c r="B64" s="4"/>
       <c r="D64" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H64" s="6"/>
       <c r="J64" s="2">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10">
       <c r="B65" s="4"/>
       <c r="D65" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F65" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H65" s="6"/>
       <c r="J65" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10">
       <c r="B66" s="4"/>
       <c r="D66" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F66" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H66" s="6"/>
       <c r="J66" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10">
       <c r="B67" s="4"/>
       <c r="D67" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F67" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H67" s="6"/>
       <c r="J67" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10">
       <c r="B68" s="4"/>
       <c r="D68" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F68" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H68" s="6"/>
       <c r="J68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10">
       <c r="B69" s="4"/>
       <c r="D69" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F69" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H69" s="6"/>
       <c r="J69" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10">
       <c r="B70" s="4"/>
       <c r="D70" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F70" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H70" s="6"/>
       <c r="J70" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10">
       <c r="B71" s="4"/>
       <c r="D71" s="5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F71" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H71" s="6"/>
       <c r="J71" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="B72" s="4"/>
+      <c r="D72" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F72" t="s">
+        <v>91</v>
+      </c>
+      <c r="H72" s="6"/>
+      <c r="J72" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="B73" s="4"/>
+      <c r="D73" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F73" t="s">
+        <v>92</v>
+      </c>
+      <c r="H73" s="6"/>
+      <c r="J73" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10">
+      <c r="B74" s="4"/>
+      <c r="D74" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74" t="s">
+        <v>93</v>
+      </c>
+      <c r="H74" s="6"/>
+      <c r="J74" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7"/>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="J72" s="7"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" t="s">
-        <v>88</v>
+    <row r="75" spans="2:10">
+      <c r="B75" s="4"/>
+      <c r="D75" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" t="s">
+        <v>94</v>
+      </c>
+      <c r="H75" s="6"/>
+      <c r="J75" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10">
+      <c r="B76" s="4"/>
+      <c r="D76" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F76" t="s">
+        <v>95</v>
+      </c>
+      <c r="H76" s="6"/>
+      <c r="J76" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10">
+      <c r="B77" s="4"/>
+      <c r="D77" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F77" t="s">
+        <v>96</v>
+      </c>
+      <c r="H77" s="6"/>
+      <c r="J77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10">
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>